<commit_message>
20150113 +++++++ cs-厂商 end ++ end +
</commit_message>
<xml_diff>
--- a/陈瑜页面对照表.xlsx
+++ b/陈瑜页面对照表.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>cs-厂商</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -65,6 +65,70 @@
   </si>
   <si>
     <t>pay_failed.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>我的收藏-店铺</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>我的收藏-商品</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>collect-store.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>collect-comm.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>我的地址</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>my-site.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>我的地址-收货地址修改</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>site-change.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>我的地址-添加地址</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>site-add.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bill.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bill-add.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>发票</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新增发票</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>意见反馈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>opinion.html</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -426,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -497,6 +561,70 @@
         <v>12</v>
       </c>
     </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
2015021 add null.html +++
</commit_message>
<xml_diff>
--- a/陈瑜页面对照表.xlsx
+++ b/陈瑜页面对照表.xlsx
@@ -356,28 +356,29 @@
     <t>申请开店</t>
   </si>
   <si>
+    <t>申请开店 -昵称设置</t>
+  </si>
+  <si>
+    <t>sus-apply-two.html</t>
+  </si>
+  <si>
+    <t>my-entrepot.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>safety-ver.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>搜索结果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>search-result.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>sus-apply.html</t>
-  </si>
-  <si>
-    <t>申请开店 -昵称设置</t>
-  </si>
-  <si>
-    <t>sus-apply-two.html</t>
-  </si>
-  <si>
-    <t>my-entrepot.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>safety-ver.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>搜索结果</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>search-result.html</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -735,8 +736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -926,10 +927,10 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="22.5">
@@ -989,7 +990,7 @@
       <c r="A34" t="s">
         <v>46</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="2" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1053,7 +1054,7 @@
         <v>71</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1125,7 +1126,7 @@
         <v>88</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -1133,15 +1134,15 @@
         <v>89</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B55" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>